<commit_message>
feat: new params to Config.xlsx
</commit_message>
<xml_diff>
--- a/Ui Path Logic/Data/Config.xlsx
+++ b/Ui Path Logic/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rique\OneDrive\Documentos\UiPath\Roit_automation_project\Ui Path Logic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561492A4-38D3-4B46-9BD0-8BB68E4A2D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BC99E0-5384-4BBB-BF57-67EFFA630267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,53 @@
   </si>
   <si>
     <t>https://cnae.ibge.gov.br/?view=estrutura</t>
+  </si>
+  <si>
+    <t>Url to the site.</t>
+  </si>
+  <si>
+    <t>PythonExe</t>
+  </si>
+  <si>
+    <t>PythonScriptPath</t>
+  </si>
+  <si>
+    <t>Excel file name to output.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Local path to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Python.</t>
+    </r>
+  </si>
+  <si>
+    <t>Path to venv and Python script.</t>
+  </si>
+  <si>
+    <t>OutputFilePath</t>
+  </si>
+  <si>
+    <t>C:\Users\rique\OneDrive\Documentos\UiPath\Roit_automation_project\Python Logic</t>
+  </si>
+  <si>
+    <t>../Ui Path Logic/CNAE_Details</t>
+  </si>
+  <si>
+    <t>C:\Users\rique\AppData\Local\Programs\Python\Python39</t>
+  </si>
+  <si>
+    <t>DirectoryPath</t>
+  </si>
+  <si>
+    <t>C:\Users\rique\OneDrive\Documentos\UiPath\Roit_automation_project\Ui Path Logic</t>
   </si>
 </sst>
 </file>
@@ -552,15 +599,16 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="75.140625" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -637,34 +685,90 @@
       <c r="B7" t="s">
         <v>46</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B10" s="5"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
fix: insert and treath data moved to 'Process.xaml'
</commit_message>
<xml_diff>
--- a/Ui Path Logic/Data/Config.xlsx
+++ b/Ui Path Logic/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rique\OneDrive\Documentos\UiPath\Roit_automation_project\Ui Path Logic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BC99E0-5384-4BBB-BF57-67EFFA630267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4728A527-5CD0-4A0E-B6AE-0C2E975F6955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,13 +599,13 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="75.140625" customWidth="1"/>
+    <col min="2" max="2" width="79.7109375" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="26" width="8.7109375" customWidth="1"/>
@@ -739,7 +739,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B16" s="2"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="5"/>

</xml_diff>